<commit_message>
GIJoe - Title screen stuff done
</commit_message>
<xml_diff>
--- a/GIJoe/GIJoe.xlsx
+++ b/GIJoe/GIJoe.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,12 +14,12 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="221">
   <si>
     <t>Notes</t>
   </si>
@@ -705,6 +705,24 @@
   <si>
     <t>adelikat, Cardboard, DarkKobold, mmbossman</t>
   </si>
+  <si>
+    <t>Level 1 Begin</t>
+  </si>
+  <si>
+    <t>Logo end</t>
+  </si>
+  <si>
+    <t>Title screen end</t>
+  </si>
+  <si>
+    <t>End map</t>
+  </si>
+  <si>
+    <t>Convo end</t>
+  </si>
+  <si>
+    <t>Route 1 end</t>
+  </si>
 </sst>
 </file>
 
@@ -714,10 +732,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1622,34 +1647,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1657,208 +1682,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1868,10 +1893,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1892,133 +1917,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2327,11 +2355,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2359,7 +2387,7 @@
       <c r="F1" s="155"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65535)</f>
+        <f>SUM(G1:G65536)</f>
         <v>0</v>
       </c>
       <c r="I1" s="141" t="s">
@@ -2498,27 +2526,43 @@
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
+      <c r="C9" s="99">
+        <v>0</v>
+      </c>
+      <c r="D9" s="99">
+        <v>0</v>
+      </c>
       <c r="E9" s="99"/>
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A10" s="149"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
+      <c r="B10" s="212" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="101">
+        <v>270</v>
+      </c>
+      <c r="D10" s="101">
+        <v>270</v>
+      </c>
       <c r="E10" s="101">
-        <f t="shared" ref="E10:E16" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
+        <f t="shared" ref="E10:E17" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
         <v>0</v>
       </c>
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
       <c r="A11" s="149"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
+      <c r="B11" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="101">
+        <v>816</v>
+      </c>
+      <c r="D11" s="101">
+        <v>816</v>
+      </c>
       <c r="E11" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2527,9 +2571,15 @@
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
       <c r="A12" s="149"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
+      <c r="B12" s="212" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="101">
+        <v>897</v>
+      </c>
+      <c r="D12" s="101">
+        <v>897</v>
+      </c>
       <c r="E12" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2538,9 +2588,15 @@
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
       <c r="A13" s="149"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
+      <c r="B13" s="212" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="101">
+        <v>942</v>
+      </c>
+      <c r="D13" s="101">
+        <v>942</v>
+      </c>
       <c r="E13" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2549,9 +2605,15 @@
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
       <c r="A14" s="149"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
+      <c r="B14" s="212" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="101">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="101">
+        <v>1000</v>
+      </c>
       <c r="E14" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2563,111 +2625,121 @@
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
-      <c r="E15" s="121">
+      <c r="E15" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="105"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="16" spans="1:11" ht="15" outlineLevel="1">
       <c r="A16" s="149"/>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="212" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101">
+        <v>1017</v>
+      </c>
+      <c r="E16" s="121">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="105"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A17" s="149"/>
+      <c r="B17" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C16" s="99">
-        <v>0</v>
-      </c>
-      <c r="D16" s="99">
-        <v>0</v>
-      </c>
-      <c r="E16" s="101">
+      <c r="C17" s="99">
+        <v>0</v>
+      </c>
+      <c r="D17" s="99">
+        <v>1017</v>
+      </c>
+      <c r="E17" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="104"/>
-    </row>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A17" s="116" t="s">
+      <c r="F17" s="104"/>
+    </row>
+    <row r="18" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A18" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="102" t="s">
+      <c r="B18" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="C17" s="103">
-        <f>C16-C9</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="103">
-        <f>D16-D9</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="122">
-        <f>E16-E9</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="112">
-        <f>E17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A19" s="150" t="s">
+      <c r="C18" s="103">
+        <f>C17-C9</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="103">
+        <f>D17-D9</f>
+        <v>1017</v>
+      </c>
+      <c r="E18" s="122">
+        <f>E17-E9</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="106"/>
+      <c r="G18" s="112">
+        <f>E18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="20" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A20" s="150" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B20" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C20" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="110" t="s">
+      <c r="D20" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="110" t="s">
+      <c r="E20" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="111" t="s">
+      <c r="F20" s="111" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A20" s="149"/>
-      <c r="B20" s="98" t="s">
+    <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A21" s="149"/>
+      <c r="B21" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="123">
-        <f t="shared" ref="E20:E33" si="1">IF(AND(C20&gt;0,D20&gt;0), D20-C20, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="104"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A21" s="149"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="124">
+      <c r="C21" s="99"/>
+      <c r="D21" s="99">
+        <v>1017</v>
+      </c>
+      <c r="E21" s="123">
+        <f t="shared" ref="E21:E34" si="1">IF(AND(C21&gt;0,D21&gt;0), D21-C21, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="104"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
+      <c r="A22" s="149"/>
+      <c r="B22" s="212" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101">
+        <v>1017</v>
+      </c>
+      <c r="E22" s="124">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="105"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A22" s="149"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="123">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="F22" s="105"/>
     </row>
-    <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="23" spans="1:7" ht="15" outlineLevel="1">
       <c r="A23" s="149"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
@@ -2678,7 +2750,7 @@
       </c>
       <c r="F23" s="105"/>
     </row>
-    <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="24" spans="1:7" ht="15" outlineLevel="1">
       <c r="A24" s="149"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
@@ -2689,7 +2761,7 @@
       </c>
       <c r="F24" s="105"/>
     </row>
-    <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="25" spans="1:7" ht="15" outlineLevel="1">
       <c r="A25" s="149"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
@@ -2700,7 +2772,7 @@
       </c>
       <c r="F25" s="105"/>
     </row>
-    <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="26" spans="1:7" ht="15" outlineLevel="1">
       <c r="A26" s="149"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
@@ -2711,7 +2783,7 @@
       </c>
       <c r="F26" s="105"/>
     </row>
-    <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="27" spans="1:7" ht="15" outlineLevel="1">
       <c r="A27" s="149"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
@@ -2722,7 +2794,7 @@
       </c>
       <c r="F27" s="105"/>
     </row>
-    <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="28" spans="1:7" ht="15" outlineLevel="1">
       <c r="A28" s="149"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
@@ -2733,7 +2805,7 @@
       </c>
       <c r="F28" s="105"/>
     </row>
-    <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="29" spans="1:7" ht="15" outlineLevel="1">
       <c r="A29" s="149"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
@@ -2744,7 +2816,7 @@
       </c>
       <c r="F29" s="105"/>
     </row>
-    <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="30" spans="1:7" ht="15" outlineLevel="1">
       <c r="A30" s="149"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
@@ -2755,7 +2827,7 @@
       </c>
       <c r="F30" s="105"/>
     </row>
-    <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="31" spans="1:7" ht="15" outlineLevel="1">
       <c r="A31" s="149"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
@@ -2766,7 +2838,7 @@
       </c>
       <c r="F31" s="105"/>
     </row>
-    <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+    <row r="32" spans="1:7" ht="15" outlineLevel="1">
       <c r="A32" s="149"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
@@ -2777,95 +2849,95 @@
       </c>
       <c r="F32" s="105"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="33" spans="1:7" ht="15" outlineLevel="1">
       <c r="A33" s="149"/>
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="100"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="105"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A34" s="149"/>
+      <c r="B34" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="125">
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="125">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F33" s="104"/>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
-      <c r="A34" s="117">
+      <c r="F34" s="104"/>
+    </row>
+    <row r="35" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A35" s="117">
         <v>1</v>
       </c>
-      <c r="B34" s="102" t="s">
+      <c r="B35" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="103">
-        <f>C33-C20</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="103">
-        <f>D33-D20</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="126">
-        <f>E33-E20</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="108"/>
-      <c r="G34" s="112">
-        <f>E34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A36" s="148" t="s">
+      <c r="C35" s="103">
+        <f>C34-C21</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="103">
+        <f>D34-D21</f>
+        <v>-1017</v>
+      </c>
+      <c r="E35" s="126">
+        <f>E34-E21</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="108"/>
+      <c r="G35" s="112">
+        <f>E35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="37" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A37" s="148" t="s">
         <v>170</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B37" s="113" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="114" t="s">
+      <c r="C37" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="114" t="s">
+      <c r="D37" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="114" t="s">
+      <c r="E37" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="115" t="s">
+      <c r="F37" s="115" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A37" s="149"/>
-      <c r="B37" s="98" t="s">
+    <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A38" s="149"/>
+      <c r="B38" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="123">
-        <f t="shared" ref="E37:E50" si="2">IF(AND(C37&gt;0,D37&gt;0), D37-C37, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="104"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A38" s="149"/>
-      <c r="B38" s="100"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="124">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="105"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C38" s="99"/>
+      <c r="D38" s="99"/>
+      <c r="E38" s="123">
+        <f t="shared" ref="E38:E51" si="2">IF(AND(C38&gt;0,D38&gt;0), D38-C38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="104"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A39" s="149"/>
       <c r="B39" s="100"/>
       <c r="C39" s="101"/>
       <c r="D39" s="101"/>
-      <c r="E39" s="123">
+      <c r="E39" s="124">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2981,95 +3053,95 @@
       </c>
       <c r="F49" s="105"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A50" s="149"/>
-      <c r="B50" s="98" t="s">
+      <c r="B50" s="100"/>
+      <c r="C50" s="101"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="105"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A51" s="149"/>
+      <c r="B51" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="125">
+      <c r="C51" s="99"/>
+      <c r="D51" s="99"/>
+      <c r="E51" s="125">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F50" s="104"/>
-    </row>
-    <row r="51" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
-      <c r="A51" s="116">
+      <c r="F51" s="104"/>
+    </row>
+    <row r="52" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+      <c r="A52" s="116">
         <v>2</v>
       </c>
-      <c r="B51" s="102" t="s">
+      <c r="B52" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C51" s="103">
-        <f>C50-C37</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="103">
-        <f>D50-D37</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="126">
-        <f>E50-E37</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="107"/>
-      <c r="G51" s="112">
-        <f>E51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A53" s="150" t="s">
+      <c r="C52" s="103">
+        <f>C51-C38</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="103">
+        <f>D51-D38</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="126">
+        <f>E51-E38</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="107"/>
+      <c r="G52" s="112">
+        <f>E52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="54" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A54" s="150" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="109" t="s">
+      <c r="B54" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="C53" s="110" t="s">
+      <c r="C54" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="110" t="s">
+      <c r="D54" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="110" t="s">
+      <c r="E54" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="111" t="s">
+      <c r="F54" s="111" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A54" s="149"/>
-      <c r="B54" s="98" t="s">
+    <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A55" s="149"/>
+      <c r="B55" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="123">
-        <f t="shared" ref="E54:E67" si="3">IF(AND(C54&gt;0,D54&gt;0), D54-C54, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="104"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A55" s="149"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="124">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="105"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C55" s="99"/>
+      <c r="D55" s="99"/>
+      <c r="E55" s="123">
+        <f t="shared" ref="E55:E68" si="3">IF(AND(C55&gt;0,D55&gt;0), D55-C55, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="104"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A56" s="149"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
-      <c r="E56" s="123">
+      <c r="E56" s="124">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3185,95 +3257,95 @@
       </c>
       <c r="F66" s="105"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="67" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A67" s="149"/>
-      <c r="B67" s="98" t="s">
+      <c r="B67" s="100"/>
+      <c r="C67" s="101"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="105"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A68" s="149"/>
+      <c r="B68" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="125">
+      <c r="C68" s="99"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="125">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F67" s="104"/>
-    </row>
-    <row r="68" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
-      <c r="A68" s="117">
+      <c r="F68" s="104"/>
+    </row>
+    <row r="69" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+      <c r="A69" s="117">
         <v>3</v>
       </c>
-      <c r="B68" s="102" t="s">
+      <c r="B69" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C68" s="103">
-        <f>C67-C54</f>
-        <v>0</v>
-      </c>
-      <c r="D68" s="103">
-        <f>D67-D54</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="126">
-        <f>E67-E54</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="108"/>
-      <c r="G68" s="112">
-        <f>E68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A70" s="148" t="s">
+      <c r="C69" s="103">
+        <f>C68-C55</f>
+        <v>0</v>
+      </c>
+      <c r="D69" s="103">
+        <f>D68-D55</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="126">
+        <f>E68-E55</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="108"/>
+      <c r="G69" s="112">
+        <f>E69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="71" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A71" s="148" t="s">
         <v>172</v>
       </c>
-      <c r="B70" s="113" t="s">
+      <c r="B71" s="113" t="s">
         <v>182</v>
       </c>
-      <c r="C70" s="114" t="s">
+      <c r="C71" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="114" t="s">
+      <c r="D71" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="114" t="s">
+      <c r="E71" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F70" s="115" t="s">
+      <c r="F71" s="115" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A71" s="149"/>
-      <c r="B71" s="98" t="s">
+    <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A72" s="149"/>
+      <c r="B72" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="99"/>
-      <c r="D71" s="99"/>
-      <c r="E71" s="123">
-        <f t="shared" ref="E71:E84" si="4">IF(AND(C71&gt;0,D71&gt;0), D71-C71, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F71" s="104"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A72" s="149"/>
-      <c r="B72" s="100"/>
-      <c r="C72" s="101"/>
-      <c r="D72" s="101"/>
-      <c r="E72" s="124">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F72" s="105"/>
-    </row>
-    <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C72" s="99"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="123">
+        <f t="shared" ref="E72:E85" si="4">IF(AND(C72&gt;0,D72&gt;0), D72-C72, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="104"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A73" s="149"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
-      <c r="E73" s="123">
+      <c r="E73" s="124">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3389,95 +3461,95 @@
       </c>
       <c r="F83" s="105"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A84" s="149"/>
-      <c r="B84" s="98" t="s">
+      <c r="B84" s="100"/>
+      <c r="C84" s="101"/>
+      <c r="D84" s="101"/>
+      <c r="E84" s="123">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F84" s="105"/>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A85" s="149"/>
+      <c r="B85" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C84" s="99"/>
-      <c r="D84" s="99"/>
-      <c r="E84" s="125">
+      <c r="C85" s="99"/>
+      <c r="D85" s="99"/>
+      <c r="E85" s="125">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F84" s="104"/>
-    </row>
-    <row r="85" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
-      <c r="A85" s="116">
+      <c r="F85" s="104"/>
+    </row>
+    <row r="86" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+      <c r="A86" s="116">
         <v>4</v>
       </c>
-      <c r="B85" s="102" t="s">
+      <c r="B86" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C85" s="103">
-        <f>C84-C71</f>
-        <v>0</v>
-      </c>
-      <c r="D85" s="103">
-        <f>D84-D71</f>
-        <v>0</v>
-      </c>
-      <c r="E85" s="126">
-        <f>E84-E71</f>
-        <v>0</v>
-      </c>
-      <c r="F85" s="107"/>
-      <c r="G85" s="112">
-        <f>E85</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A87" s="150" t="s">
+      <c r="C86" s="103">
+        <f>C85-C72</f>
+        <v>0</v>
+      </c>
+      <c r="D86" s="103">
+        <f>D85-D72</f>
+        <v>0</v>
+      </c>
+      <c r="E86" s="126">
+        <f>E85-E72</f>
+        <v>0</v>
+      </c>
+      <c r="F86" s="107"/>
+      <c r="G86" s="112">
+        <f>E86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="88" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A88" s="150" t="s">
         <v>173</v>
       </c>
-      <c r="B87" s="109" t="s">
+      <c r="B88" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="C87" s="110" t="s">
+      <c r="C88" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D87" s="110" t="s">
+      <c r="D88" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E87" s="110" t="s">
+      <c r="E88" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F87" s="111" t="s">
+      <c r="F88" s="111" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A88" s="149"/>
-      <c r="B88" s="98" t="s">
+    <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A89" s="149"/>
+      <c r="B89" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C88" s="99"/>
-      <c r="D88" s="99"/>
-      <c r="E88" s="123">
-        <f t="shared" ref="E88:E101" si="5">IF(AND(C88&gt;0,D88&gt;0), D88-C88, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F88" s="104"/>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A89" s="149"/>
-      <c r="B89" s="100"/>
-      <c r="C89" s="101"/>
-      <c r="D89" s="101"/>
-      <c r="E89" s="124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F89" s="105"/>
-    </row>
-    <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C89" s="99"/>
+      <c r="D89" s="99"/>
+      <c r="E89" s="123">
+        <f t="shared" ref="E89:E102" si="5">IF(AND(C89&gt;0,D89&gt;0), D89-C89, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F89" s="104"/>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A90" s="149"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
-      <c r="E90" s="123">
+      <c r="E90" s="124">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3593,94 +3665,94 @@
       </c>
       <c r="F100" s="105"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A101" s="149"/>
-      <c r="B101" s="98" t="s">
+      <c r="B101" s="100"/>
+      <c r="C101" s="101"/>
+      <c r="D101" s="101"/>
+      <c r="E101" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F101" s="105"/>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A102" s="149"/>
+      <c r="B102" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C101" s="99"/>
-      <c r="D101" s="99"/>
-      <c r="E101" s="125">
+      <c r="C102" s="99"/>
+      <c r="D102" s="99"/>
+      <c r="E102" s="125">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F101" s="104"/>
-    </row>
-    <row r="102" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
-      <c r="A102" s="117">
+      <c r="F102" s="104"/>
+    </row>
+    <row r="103" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1">
+      <c r="A103" s="117">
         <v>5</v>
       </c>
-      <c r="B102" s="102" t="s">
+      <c r="B103" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C102" s="103">
-        <f>C101-C88</f>
-        <v>0</v>
-      </c>
-      <c r="D102" s="103">
-        <f>D101-D88</f>
-        <v>0</v>
-      </c>
-      <c r="E102" s="126">
-        <f>E101-E88</f>
-        <v>0</v>
-      </c>
-      <c r="F102" s="108"/>
-      <c r="G102" s="112">
-        <f>E102</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A104" s="148" t="s">
+      <c r="C103" s="103">
+        <f>C102-C89</f>
+        <v>0</v>
+      </c>
+      <c r="D103" s="103">
+        <f>D102-D89</f>
+        <v>0</v>
+      </c>
+      <c r="E103" s="126">
+        <f>E102-E89</f>
+        <v>0</v>
+      </c>
+      <c r="F103" s="108"/>
+      <c r="G103" s="112">
+        <f>E103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="A105" s="148" t="s">
         <v>174</v>
       </c>
-      <c r="B104" s="113" t="s">
+      <c r="B105" s="113" t="s">
         <v>182</v>
       </c>
-      <c r="C104" s="114" t="s">
+      <c r="C105" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D104" s="114" t="s">
+      <c r="D105" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E104" s="114" t="s">
+      <c r="E105" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F104" s="115" t="s">
+      <c r="F105" s="115" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A105" s="149"/>
-      <c r="B105" s="98" t="s">
+    <row r="106" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A106" s="149"/>
+      <c r="B106" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C105" s="99"/>
-      <c r="D105" s="99"/>
-      <c r="E105" s="123">
-        <f t="shared" ref="E105:E118" si="6">IF(AND(C105&gt;0,D105&gt;0), D105-C105, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F105" s="104"/>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A106" s="149"/>
-      <c r="B106" s="100"/>
-      <c r="C106" s="101"/>
-      <c r="D106" s="101"/>
-      <c r="E106" s="124">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F106" s="105"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C106" s="99"/>
+      <c r="D106" s="99"/>
+      <c r="E106" s="123">
+        <f t="shared" ref="E106:E119" si="6">IF(AND(C106&gt;0,D106&gt;0), D106-C106, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F106" s="104"/>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A107" s="149"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
-      <c r="E107" s="123">
+      <c r="E107" s="124">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3796,94 +3868,94 @@
       </c>
       <c r="F117" s="105"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A118" s="149"/>
-      <c r="B118" s="98" t="s">
+      <c r="B118" s="100"/>
+      <c r="C118" s="101"/>
+      <c r="D118" s="101"/>
+      <c r="E118" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="105"/>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A119" s="149"/>
+      <c r="B119" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C118" s="99"/>
-      <c r="D118" s="99"/>
-      <c r="E118" s="125">
+      <c r="C119" s="99"/>
+      <c r="D119" s="99"/>
+      <c r="E119" s="125">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F118" s="104"/>
-    </row>
-    <row r="119" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A119" s="116">
+      <c r="F119" s="104"/>
+    </row>
+    <row r="120" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A120" s="116">
         <v>6</v>
       </c>
-      <c r="B119" s="102" t="s">
+      <c r="B120" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C119" s="103">
-        <f>C118-C105</f>
-        <v>0</v>
-      </c>
-      <c r="D119" s="103">
-        <f>D118-D105</f>
-        <v>0</v>
-      </c>
-      <c r="E119" s="103">
-        <f>E118-E105</f>
-        <v>0</v>
-      </c>
-      <c r="F119" s="107"/>
-      <c r="G119" s="112">
-        <f>E119</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A121" s="150" t="s">
+      <c r="C120" s="103">
+        <f>C119-C106</f>
+        <v>0</v>
+      </c>
+      <c r="D120" s="103">
+        <f>D119-D106</f>
+        <v>0</v>
+      </c>
+      <c r="E120" s="103">
+        <f>E119-E106</f>
+        <v>0</v>
+      </c>
+      <c r="F120" s="107"/>
+      <c r="G120" s="112">
+        <f>E120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="A122" s="150" t="s">
         <v>175</v>
       </c>
-      <c r="B121" s="109" t="s">
+      <c r="B122" s="109" t="s">
         <v>182</v>
       </c>
-      <c r="C121" s="110" t="s">
+      <c r="C122" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D121" s="110" t="s">
+      <c r="D122" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E121" s="110" t="s">
+      <c r="E122" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F121" s="111" t="s">
+      <c r="F122" s="111" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A122" s="149"/>
-      <c r="B122" s="98" t="s">
+    <row r="123" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A123" s="149"/>
+      <c r="B123" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C122" s="99"/>
-      <c r="D122" s="99"/>
-      <c r="E122" s="123">
-        <f t="shared" ref="E122:E135" si="7">IF(AND(C122&gt;0,D122&gt;0), D122-C122, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F122" s="104"/>
-    </row>
-    <row r="123" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A123" s="149"/>
-      <c r="B123" s="100"/>
-      <c r="C123" s="101"/>
-      <c r="D123" s="101"/>
-      <c r="E123" s="124">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F123" s="105"/>
-    </row>
-    <row r="124" spans="1:7" ht="15" hidden="1" outlineLevel="1">
+      <c r="C123" s="99"/>
+      <c r="D123" s="99"/>
+      <c r="E123" s="123">
+        <f t="shared" ref="E123:E136" si="7">IF(AND(C123&gt;0,D123&gt;0), D123-C123, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F123" s="104"/>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A124" s="149"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
-      <c r="E124" s="123">
+      <c r="E124" s="124">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3999,94 +4071,94 @@
       </c>
       <c r="F134" s="105"/>
     </row>
-    <row r="135" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1">
       <c r="A135" s="149"/>
-      <c r="B135" s="98" t="s">
+      <c r="B135" s="100"/>
+      <c r="C135" s="101"/>
+      <c r="D135" s="101"/>
+      <c r="E135" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F135" s="105"/>
+    </row>
+    <row r="136" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A136" s="149"/>
+      <c r="B136" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C135" s="99"/>
-      <c r="D135" s="99"/>
-      <c r="E135" s="125">
+      <c r="C136" s="99"/>
+      <c r="D136" s="99"/>
+      <c r="E136" s="125">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F135" s="104"/>
-    </row>
-    <row r="136" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A136" s="117">
+      <c r="F136" s="104"/>
+    </row>
+    <row r="137" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A137" s="117">
         <v>7</v>
       </c>
-      <c r="B136" s="102" t="s">
+      <c r="B137" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C136" s="103">
-        <f>C135-C122</f>
-        <v>0</v>
-      </c>
-      <c r="D136" s="103">
-        <f>D135-D122</f>
-        <v>0</v>
-      </c>
-      <c r="E136" s="103">
-        <f>E135-E122</f>
-        <v>0</v>
-      </c>
-      <c r="F136" s="108"/>
-      <c r="G136" s="112">
-        <f>E136</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A138" s="148" t="s">
+      <c r="C137" s="103">
+        <f>C136-C123</f>
+        <v>0</v>
+      </c>
+      <c r="D137" s="103">
+        <f>D136-D123</f>
+        <v>0</v>
+      </c>
+      <c r="E137" s="103">
+        <f>E136-E123</f>
+        <v>0</v>
+      </c>
+      <c r="F137" s="108"/>
+      <c r="G137" s="112">
+        <f>E137</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+      <c r="A139" s="148" t="s">
         <v>176</v>
       </c>
-      <c r="B138" s="113" t="s">
+      <c r="B139" s="113" t="s">
         <v>182</v>
       </c>
-      <c r="C138" s="114" t="s">
+      <c r="C139" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D138" s="114" t="s">
+      <c r="D139" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E138" s="114" t="s">
+      <c r="E139" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F138" s="115" t="s">
+      <c r="F139" s="115" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A139" s="149"/>
-      <c r="B139" s="98" t="s">
+    <row r="140" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A140" s="149"/>
+      <c r="B140" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C139" s="99"/>
-      <c r="D139" s="99"/>
-      <c r="E139" s="123">
-        <f t="shared" ref="E139:E152" si="8">IF(AND(C139&gt;0,D139&gt;0), D139-C139, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F139" s="104"/>
-    </row>
-    <row r="140" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A140" s="149"/>
-      <c r="B140" s="100"/>
-      <c r="C140" s="101"/>
-      <c r="D140" s="101"/>
-      <c r="E140" s="124">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F140" s="105"/>
-    </row>
-    <row r="141" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+      <c r="C140" s="99"/>
+      <c r="D140" s="99"/>
+      <c r="E140" s="123">
+        <f t="shared" ref="E140:E153" si="8">IF(AND(C140&gt;0,D140&gt;0), D140-C140, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F140" s="104"/>
+    </row>
+    <row r="141" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
       <c r="A141" s="149"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
-      <c r="E141" s="123">
+      <c r="E141" s="124">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4202,59 +4274,70 @@
       </c>
       <c r="F151" s="105"/>
     </row>
-    <row r="152" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
       <c r="A152" s="149"/>
-      <c r="B152" s="98" t="s">
+      <c r="B152" s="100"/>
+      <c r="C152" s="101"/>
+      <c r="D152" s="101"/>
+      <c r="E152" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F152" s="105"/>
+    </row>
+    <row r="153" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A153" s="149"/>
+      <c r="B153" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C152" s="99"/>
-      <c r="D152" s="99"/>
-      <c r="E152" s="125">
+      <c r="C153" s="99"/>
+      <c r="D153" s="99"/>
+      <c r="E153" s="125">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F152" s="104"/>
-    </row>
-    <row r="153" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A153" s="116">
+      <c r="F153" s="104"/>
+    </row>
+    <row r="154" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A154" s="116">
         <v>8</v>
       </c>
-      <c r="B153" s="102" t="s">
+      <c r="B154" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C153" s="103">
-        <f>C152-C139</f>
-        <v>0</v>
-      </c>
-      <c r="D153" s="103">
-        <f>D152-D139</f>
-        <v>0</v>
-      </c>
-      <c r="E153" s="103">
-        <f>E152-E139</f>
-        <v>0</v>
-      </c>
-      <c r="F153" s="107"/>
-      <c r="G153" s="112">
-        <f>E153</f>
+      <c r="C154" s="103">
+        <f>C153-C140</f>
+        <v>0</v>
+      </c>
+      <c r="D154" s="103">
+        <f>D153-D140</f>
+        <v>0</v>
+      </c>
+      <c r="E154" s="103">
+        <f>E153-E140</f>
+        <v>0</v>
+      </c>
+      <c r="F154" s="107"/>
+      <c r="G154" s="112">
+        <f>E154</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A138:A152"/>
-    <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="A37:A51"/>
+    <mergeCell ref="A54:A68"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="A20:A34"/>
+    <mergeCell ref="A139:A153"/>
+    <mergeCell ref="A105:A119"/>
+    <mergeCell ref="A71:A85"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A88:A102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4286,13 +4369,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="175" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4322,18 +4405,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4485,9 +4568,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="162"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="160"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4638,9 +4721,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
+      <c r="C38" s="157"/>
+      <c r="D38" s="158"/>
+      <c r="E38" s="158"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -4791,9 +4874,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="161"/>
+      <c r="C55" s="157"/>
+      <c r="D55" s="158"/>
+      <c r="E55" s="158"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -4944,9 +5027,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="160"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="161"/>
+      <c r="C72" s="157"/>
+      <c r="D72" s="158"/>
+      <c r="E72" s="158"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5097,9 +5180,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="161"/>
-      <c r="E89" s="161"/>
+      <c r="C89" s="157"/>
+      <c r="D89" s="158"/>
+      <c r="E89" s="158"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5250,9 +5333,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="160"/>
-      <c r="D106" s="161"/>
-      <c r="E106" s="161"/>
+      <c r="C106" s="157"/>
+      <c r="D106" s="158"/>
+      <c r="E106" s="158"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5403,9 +5486,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="160"/>
-      <c r="D123" s="161"/>
-      <c r="E123" s="161"/>
+      <c r="C123" s="157"/>
+      <c r="D123" s="158"/>
+      <c r="E123" s="158"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5556,9 +5639,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="160"/>
-      <c r="D140" s="161"/>
-      <c r="E140" s="161"/>
+      <c r="C140" s="157"/>
+      <c r="D140" s="158"/>
+      <c r="E140" s="158"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5709,9 +5792,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="160"/>
-      <c r="D157" s="161"/>
-      <c r="E157" s="161"/>
+      <c r="C157" s="157"/>
+      <c r="D157" s="158"/>
+      <c r="E157" s="158"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -5862,9 +5945,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="160"/>
-      <c r="D174" s="161"/>
-      <c r="E174" s="161"/>
+      <c r="C174" s="157"/>
+      <c r="D174" s="158"/>
+      <c r="E174" s="158"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6015,9 +6098,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="160"/>
-      <c r="D191" s="161"/>
-      <c r="E191" s="161"/>
+      <c r="C191" s="157"/>
+      <c r="D191" s="158"/>
+      <c r="E191" s="158"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6168,9 +6251,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="160"/>
-      <c r="D208" s="161"/>
-      <c r="E208" s="161"/>
+      <c r="C208" s="157"/>
+      <c r="D208" s="158"/>
+      <c r="E208" s="158"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6321,9 +6404,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="160"/>
-      <c r="D225" s="161"/>
-      <c r="E225" s="161"/>
+      <c r="C225" s="157"/>
+      <c r="D225" s="158"/>
+      <c r="E225" s="158"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6474,9 +6557,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="160"/>
-      <c r="D242" s="161"/>
-      <c r="E242" s="161"/>
+      <c r="C242" s="157"/>
+      <c r="D242" s="158"/>
+      <c r="E242" s="158"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6627,9 +6710,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="160"/>
-      <c r="D259" s="161"/>
-      <c r="E259" s="161"/>
+      <c r="C259" s="157"/>
+      <c r="D259" s="158"/>
+      <c r="E259" s="158"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -6780,18 +6863,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="164"/>
-      <c r="D276" s="165"/>
-      <c r="E276" s="165"/>
+      <c r="C276" s="173"/>
+      <c r="D276" s="174"/>
+      <c r="E276" s="174"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="160"/>
-      <c r="D277" s="161"/>
-      <c r="E277" s="161"/>
+      <c r="C277" s="157"/>
+      <c r="D277" s="158"/>
+      <c r="E277" s="158"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -6942,9 +7025,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="162"/>
-      <c r="D294" s="163"/>
-      <c r="E294" s="163"/>
+      <c r="C294" s="159"/>
+      <c r="D294" s="160"/>
+      <c r="E294" s="160"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7095,9 +7178,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="160"/>
-      <c r="D311" s="161"/>
-      <c r="E311" s="161"/>
+      <c r="C311" s="157"/>
+      <c r="D311" s="158"/>
+      <c r="E311" s="158"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7248,9 +7331,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="160"/>
-      <c r="D328" s="161"/>
-      <c r="E328" s="161"/>
+      <c r="C328" s="157"/>
+      <c r="D328" s="158"/>
+      <c r="E328" s="158"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7401,9 +7484,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="160"/>
-      <c r="D345" s="161"/>
-      <c r="E345" s="161"/>
+      <c r="C345" s="157"/>
+      <c r="D345" s="158"/>
+      <c r="E345" s="158"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7554,9 +7637,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="160"/>
-      <c r="D362" s="161"/>
-      <c r="E362" s="161"/>
+      <c r="C362" s="157"/>
+      <c r="D362" s="158"/>
+      <c r="E362" s="158"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7707,9 +7790,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="160"/>
-      <c r="D379" s="161"/>
-      <c r="E379" s="161"/>
+      <c r="C379" s="157"/>
+      <c r="D379" s="158"/>
+      <c r="E379" s="158"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -7860,9 +7943,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="160"/>
-      <c r="D396" s="161"/>
-      <c r="E396" s="161"/>
+      <c r="C396" s="157"/>
+      <c r="D396" s="158"/>
+      <c r="E396" s="158"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8013,9 +8096,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="160"/>
-      <c r="D413" s="161"/>
-      <c r="E413" s="161"/>
+      <c r="C413" s="157"/>
+      <c r="D413" s="158"/>
+      <c r="E413" s="158"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8166,9 +8249,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="160"/>
-      <c r="D430" s="161"/>
-      <c r="E430" s="161"/>
+      <c r="C430" s="157"/>
+      <c r="D430" s="158"/>
+      <c r="E430" s="158"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8319,9 +8402,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="160"/>
-      <c r="D447" s="161"/>
-      <c r="E447" s="161"/>
+      <c r="C447" s="157"/>
+      <c r="D447" s="158"/>
+      <c r="E447" s="158"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8472,9 +8555,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="160"/>
-      <c r="D464" s="161"/>
-      <c r="E464" s="161"/>
+      <c r="C464" s="157"/>
+      <c r="D464" s="158"/>
+      <c r="E464" s="158"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8625,9 +8708,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="160"/>
-      <c r="D481" s="161"/>
-      <c r="E481" s="161"/>
+      <c r="C481" s="157"/>
+      <c r="D481" s="158"/>
+      <c r="E481" s="158"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -8778,9 +8861,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="160"/>
-      <c r="D498" s="161"/>
-      <c r="E498" s="161"/>
+      <c r="C498" s="157"/>
+      <c r="D498" s="158"/>
+      <c r="E498" s="158"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -8931,9 +9014,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="160"/>
-      <c r="D515" s="161"/>
-      <c r="E515" s="161"/>
+      <c r="C515" s="157"/>
+      <c r="D515" s="158"/>
+      <c r="E515" s="158"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9084,9 +9167,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="160"/>
-      <c r="D532" s="161"/>
-      <c r="E532" s="161"/>
+      <c r="C532" s="157"/>
+      <c r="D532" s="158"/>
+      <c r="E532" s="158"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9237,18 +9320,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="166"/>
-      <c r="D549" s="167"/>
-      <c r="E549" s="167"/>
+      <c r="C549" s="171"/>
+      <c r="D549" s="172"/>
+      <c r="E549" s="172"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="160"/>
-      <c r="D550" s="161"/>
-      <c r="E550" s="161"/>
+      <c r="C550" s="157"/>
+      <c r="D550" s="158"/>
+      <c r="E550" s="158"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9399,9 +9482,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="162"/>
-      <c r="D567" s="163"/>
-      <c r="E567" s="163"/>
+      <c r="C567" s="159"/>
+      <c r="D567" s="160"/>
+      <c r="E567" s="160"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9552,9 +9635,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="160"/>
-      <c r="D584" s="161"/>
-      <c r="E584" s="161"/>
+      <c r="C584" s="157"/>
+      <c r="D584" s="158"/>
+      <c r="E584" s="158"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9705,9 +9788,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="160"/>
-      <c r="D601" s="161"/>
-      <c r="E601" s="161"/>
+      <c r="C601" s="157"/>
+      <c r="D601" s="158"/>
+      <c r="E601" s="158"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -9858,9 +9941,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="160"/>
-      <c r="D618" s="161"/>
-      <c r="E618" s="161"/>
+      <c r="C618" s="157"/>
+      <c r="D618" s="158"/>
+      <c r="E618" s="158"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10011,9 +10094,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="160"/>
-      <c r="D635" s="161"/>
-      <c r="E635" s="161"/>
+      <c r="C635" s="157"/>
+      <c r="D635" s="158"/>
+      <c r="E635" s="158"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10164,9 +10247,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="160"/>
-      <c r="D652" s="161"/>
-      <c r="E652" s="161"/>
+      <c r="C652" s="157"/>
+      <c r="D652" s="158"/>
+      <c r="E652" s="158"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10317,9 +10400,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="160"/>
-      <c r="D669" s="161"/>
-      <c r="E669" s="161"/>
+      <c r="C669" s="157"/>
+      <c r="D669" s="158"/>
+      <c r="E669" s="158"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10470,9 +10553,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="160"/>
-      <c r="D686" s="161"/>
-      <c r="E686" s="161"/>
+      <c r="C686" s="157"/>
+      <c r="D686" s="158"/>
+      <c r="E686" s="158"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10623,9 +10706,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="160"/>
-      <c r="D703" s="161"/>
-      <c r="E703" s="161"/>
+      <c r="C703" s="157"/>
+      <c r="D703" s="158"/>
+      <c r="E703" s="158"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -10776,9 +10859,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="160"/>
-      <c r="D720" s="161"/>
-      <c r="E720" s="161"/>
+      <c r="C720" s="157"/>
+      <c r="D720" s="158"/>
+      <c r="E720" s="158"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -10929,9 +11012,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="160"/>
-      <c r="D737" s="161"/>
-      <c r="E737" s="161"/>
+      <c r="C737" s="157"/>
+      <c r="D737" s="158"/>
+      <c r="E737" s="158"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11082,9 +11165,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="160"/>
-      <c r="D754" s="161"/>
-      <c r="E754" s="161"/>
+      <c r="C754" s="157"/>
+      <c r="D754" s="158"/>
+      <c r="E754" s="158"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11235,9 +11318,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="160"/>
-      <c r="D771" s="161"/>
-      <c r="E771" s="161"/>
+      <c r="C771" s="157"/>
+      <c r="D771" s="158"/>
+      <c r="E771" s="158"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11388,9 +11471,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="160"/>
-      <c r="D788" s="161"/>
-      <c r="E788" s="161"/>
+      <c r="C788" s="157"/>
+      <c r="D788" s="158"/>
+      <c r="E788" s="158"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11541,9 +11624,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="160"/>
-      <c r="D805" s="161"/>
-      <c r="E805" s="161"/>
+      <c r="C805" s="157"/>
+      <c r="D805" s="158"/>
+      <c r="E805" s="158"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11694,18 +11777,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="168"/>
-      <c r="D822" s="169"/>
-      <c r="E822" s="169"/>
+      <c r="C822" s="169"/>
+      <c r="D822" s="170"/>
+      <c r="E822" s="170"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="160"/>
-      <c r="D823" s="161"/>
-      <c r="E823" s="161"/>
+      <c r="C823" s="157"/>
+      <c r="D823" s="158"/>
+      <c r="E823" s="158"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -11856,9 +11939,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="162"/>
-      <c r="D840" s="163"/>
-      <c r="E840" s="163"/>
+      <c r="C840" s="159"/>
+      <c r="D840" s="160"/>
+      <c r="E840" s="160"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12009,9 +12092,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="160"/>
-      <c r="D857" s="161"/>
-      <c r="E857" s="161"/>
+      <c r="C857" s="157"/>
+      <c r="D857" s="158"/>
+      <c r="E857" s="158"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12162,9 +12245,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="160"/>
-      <c r="D874" s="161"/>
-      <c r="E874" s="161"/>
+      <c r="C874" s="157"/>
+      <c r="D874" s="158"/>
+      <c r="E874" s="158"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12315,9 +12398,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="160"/>
-      <c r="D891" s="161"/>
-      <c r="E891" s="161"/>
+      <c r="C891" s="157"/>
+      <c r="D891" s="158"/>
+      <c r="E891" s="158"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12468,9 +12551,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="160"/>
-      <c r="D908" s="161"/>
-      <c r="E908" s="161"/>
+      <c r="C908" s="157"/>
+      <c r="D908" s="158"/>
+      <c r="E908" s="158"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12621,9 +12704,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="160"/>
-      <c r="D925" s="161"/>
-      <c r="E925" s="161"/>
+      <c r="C925" s="157"/>
+      <c r="D925" s="158"/>
+      <c r="E925" s="158"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -12774,9 +12857,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="160"/>
-      <c r="D942" s="161"/>
-      <c r="E942" s="161"/>
+      <c r="C942" s="157"/>
+      <c r="D942" s="158"/>
+      <c r="E942" s="158"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -12927,9 +13010,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="160"/>
-      <c r="D959" s="161"/>
-      <c r="E959" s="161"/>
+      <c r="C959" s="157"/>
+      <c r="D959" s="158"/>
+      <c r="E959" s="158"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13080,9 +13163,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="160"/>
-      <c r="D976" s="161"/>
-      <c r="E976" s="161"/>
+      <c r="C976" s="157"/>
+      <c r="D976" s="158"/>
+      <c r="E976" s="158"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13233,9 +13316,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="160"/>
-      <c r="D993" s="161"/>
-      <c r="E993" s="161"/>
+      <c r="C993" s="157"/>
+      <c r="D993" s="158"/>
+      <c r="E993" s="158"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13386,9 +13469,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="160"/>
-      <c r="D1010" s="161"/>
-      <c r="E1010" s="161"/>
+      <c r="C1010" s="157"/>
+      <c r="D1010" s="158"/>
+      <c r="E1010" s="158"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13539,9 +13622,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="160"/>
-      <c r="D1027" s="161"/>
-      <c r="E1027" s="161"/>
+      <c r="C1027" s="157"/>
+      <c r="D1027" s="158"/>
+      <c r="E1027" s="158"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13692,9 +13775,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="160"/>
-      <c r="D1044" s="161"/>
-      <c r="E1044" s="161"/>
+      <c r="C1044" s="157"/>
+      <c r="D1044" s="158"/>
+      <c r="E1044" s="158"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -13845,9 +13928,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="160"/>
-      <c r="D1061" s="161"/>
-      <c r="E1061" s="161"/>
+      <c r="C1061" s="157"/>
+      <c r="D1061" s="158"/>
+      <c r="E1061" s="158"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -13998,9 +14081,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="160"/>
-      <c r="D1078" s="161"/>
-      <c r="E1078" s="161"/>
+      <c r="C1078" s="157"/>
+      <c r="D1078" s="158"/>
+      <c r="E1078" s="158"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14151,18 +14234,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="170"/>
-      <c r="D1095" s="171"/>
-      <c r="E1095" s="171"/>
+      <c r="C1095" s="167"/>
+      <c r="D1095" s="168"/>
+      <c r="E1095" s="168"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="160"/>
-      <c r="D1096" s="161"/>
-      <c r="E1096" s="161"/>
+      <c r="C1096" s="157"/>
+      <c r="D1096" s="158"/>
+      <c r="E1096" s="158"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14313,9 +14396,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="162"/>
-      <c r="D1113" s="163"/>
-      <c r="E1113" s="163"/>
+      <c r="C1113" s="159"/>
+      <c r="D1113" s="160"/>
+      <c r="E1113" s="160"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14466,9 +14549,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="160"/>
-      <c r="D1130" s="161"/>
-      <c r="E1130" s="161"/>
+      <c r="C1130" s="157"/>
+      <c r="D1130" s="158"/>
+      <c r="E1130" s="158"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14619,9 +14702,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="160"/>
-      <c r="D1147" s="161"/>
-      <c r="E1147" s="161"/>
+      <c r="C1147" s="157"/>
+      <c r="D1147" s="158"/>
+      <c r="E1147" s="158"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -14772,9 +14855,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="160"/>
-      <c r="D1164" s="161"/>
-      <c r="E1164" s="161"/>
+      <c r="C1164" s="157"/>
+      <c r="D1164" s="158"/>
+      <c r="E1164" s="158"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -14925,9 +15008,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="160"/>
-      <c r="D1181" s="161"/>
-      <c r="E1181" s="161"/>
+      <c r="C1181" s="157"/>
+      <c r="D1181" s="158"/>
+      <c r="E1181" s="158"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15078,9 +15161,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="160"/>
-      <c r="D1198" s="161"/>
-      <c r="E1198" s="161"/>
+      <c r="C1198" s="157"/>
+      <c r="D1198" s="158"/>
+      <c r="E1198" s="158"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15231,9 +15314,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="160"/>
-      <c r="D1215" s="161"/>
-      <c r="E1215" s="161"/>
+      <c r="C1215" s="157"/>
+      <c r="D1215" s="158"/>
+      <c r="E1215" s="158"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15384,9 +15467,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="160"/>
-      <c r="D1232" s="161"/>
-      <c r="E1232" s="161"/>
+      <c r="C1232" s="157"/>
+      <c r="D1232" s="158"/>
+      <c r="E1232" s="158"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15537,9 +15620,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="160"/>
-      <c r="D1249" s="161"/>
-      <c r="E1249" s="161"/>
+      <c r="C1249" s="157"/>
+      <c r="D1249" s="158"/>
+      <c r="E1249" s="158"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15690,9 +15773,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="160"/>
-      <c r="D1266" s="161"/>
-      <c r="E1266" s="161"/>
+      <c r="C1266" s="157"/>
+      <c r="D1266" s="158"/>
+      <c r="E1266" s="158"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -15843,9 +15926,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="160"/>
-      <c r="D1283" s="161"/>
-      <c r="E1283" s="161"/>
+      <c r="C1283" s="157"/>
+      <c r="D1283" s="158"/>
+      <c r="E1283" s="158"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -15996,9 +16079,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="160"/>
-      <c r="D1300" s="161"/>
-      <c r="E1300" s="161"/>
+      <c r="C1300" s="157"/>
+      <c r="D1300" s="158"/>
+      <c r="E1300" s="158"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16149,9 +16232,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="160"/>
-      <c r="D1317" s="161"/>
-      <c r="E1317" s="161"/>
+      <c r="C1317" s="157"/>
+      <c r="D1317" s="158"/>
+      <c r="E1317" s="158"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16302,9 +16385,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="160"/>
-      <c r="D1334" s="161"/>
-      <c r="E1334" s="161"/>
+      <c r="C1334" s="157"/>
+      <c r="D1334" s="158"/>
+      <c r="E1334" s="158"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16455,9 +16538,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="160"/>
-      <c r="D1351" s="161"/>
-      <c r="E1351" s="161"/>
+      <c r="C1351" s="157"/>
+      <c r="D1351" s="158"/>
+      <c r="E1351" s="158"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16608,18 +16691,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="165"/>
+      <c r="D1368" s="166"/>
+      <c r="E1368" s="166"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="160"/>
-      <c r="D1369" s="161"/>
-      <c r="E1369" s="161"/>
+      <c r="C1369" s="157"/>
+      <c r="D1369" s="158"/>
+      <c r="E1369" s="158"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -16770,9 +16853,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="162"/>
-      <c r="D1386" s="163"/>
-      <c r="E1386" s="163"/>
+      <c r="C1386" s="159"/>
+      <c r="D1386" s="160"/>
+      <c r="E1386" s="160"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -16923,9 +17006,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="160"/>
-      <c r="D1403" s="161"/>
-      <c r="E1403" s="161"/>
+      <c r="C1403" s="157"/>
+      <c r="D1403" s="158"/>
+      <c r="E1403" s="158"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17076,9 +17159,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="160"/>
-      <c r="D1420" s="161"/>
-      <c r="E1420" s="161"/>
+      <c r="C1420" s="157"/>
+      <c r="D1420" s="158"/>
+      <c r="E1420" s="158"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17229,9 +17312,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="160"/>
-      <c r="D1437" s="161"/>
-      <c r="E1437" s="161"/>
+      <c r="C1437" s="157"/>
+      <c r="D1437" s="158"/>
+      <c r="E1437" s="158"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17382,9 +17465,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="160"/>
-      <c r="D1454" s="161"/>
-      <c r="E1454" s="161"/>
+      <c r="C1454" s="157"/>
+      <c r="D1454" s="158"/>
+      <c r="E1454" s="158"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17535,9 +17618,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="160"/>
-      <c r="D1471" s="161"/>
-      <c r="E1471" s="161"/>
+      <c r="C1471" s="157"/>
+      <c r="D1471" s="158"/>
+      <c r="E1471" s="158"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17688,9 +17771,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="160"/>
-      <c r="D1488" s="161"/>
-      <c r="E1488" s="161"/>
+      <c r="C1488" s="157"/>
+      <c r="D1488" s="158"/>
+      <c r="E1488" s="158"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -17841,9 +17924,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="160"/>
-      <c r="D1505" s="161"/>
-      <c r="E1505" s="161"/>
+      <c r="C1505" s="157"/>
+      <c r="D1505" s="158"/>
+      <c r="E1505" s="158"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -17994,9 +18077,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="160"/>
-      <c r="D1522" s="161"/>
-      <c r="E1522" s="161"/>
+      <c r="C1522" s="157"/>
+      <c r="D1522" s="158"/>
+      <c r="E1522" s="158"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18147,9 +18230,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="160"/>
-      <c r="D1539" s="161"/>
-      <c r="E1539" s="161"/>
+      <c r="C1539" s="157"/>
+      <c r="D1539" s="158"/>
+      <c r="E1539" s="158"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18300,9 +18383,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="160"/>
-      <c r="D1556" s="161"/>
-      <c r="E1556" s="161"/>
+      <c r="C1556" s="157"/>
+      <c r="D1556" s="158"/>
+      <c r="E1556" s="158"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18453,9 +18536,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="160"/>
-      <c r="D1573" s="161"/>
-      <c r="E1573" s="161"/>
+      <c r="C1573" s="157"/>
+      <c r="D1573" s="158"/>
+      <c r="E1573" s="158"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18606,9 +18689,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="160"/>
-      <c r="D1590" s="161"/>
-      <c r="E1590" s="161"/>
+      <c r="C1590" s="157"/>
+      <c r="D1590" s="158"/>
+      <c r="E1590" s="158"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -18759,9 +18842,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="160"/>
-      <c r="D1607" s="161"/>
-      <c r="E1607" s="161"/>
+      <c r="C1607" s="157"/>
+      <c r="D1607" s="158"/>
+      <c r="E1607" s="158"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -18912,9 +18995,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="160"/>
-      <c r="D1624" s="161"/>
-      <c r="E1624" s="161"/>
+      <c r="C1624" s="157"/>
+      <c r="D1624" s="158"/>
+      <c r="E1624" s="158"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19065,18 +19148,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="174"/>
-      <c r="D1641" s="175"/>
-      <c r="E1641" s="175"/>
+      <c r="C1641" s="163"/>
+      <c r="D1641" s="164"/>
+      <c r="E1641" s="164"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="160"/>
-      <c r="D1642" s="161"/>
-      <c r="E1642" s="161"/>
+      <c r="C1642" s="157"/>
+      <c r="D1642" s="158"/>
+      <c r="E1642" s="158"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19227,9 +19310,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="162"/>
-      <c r="D1659" s="163"/>
-      <c r="E1659" s="163"/>
+      <c r="C1659" s="159"/>
+      <c r="D1659" s="160"/>
+      <c r="E1659" s="160"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19380,9 +19463,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="160"/>
-      <c r="D1676" s="161"/>
-      <c r="E1676" s="161"/>
+      <c r="C1676" s="157"/>
+      <c r="D1676" s="158"/>
+      <c r="E1676" s="158"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19533,9 +19616,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="160"/>
-      <c r="D1693" s="161"/>
-      <c r="E1693" s="161"/>
+      <c r="C1693" s="157"/>
+      <c r="D1693" s="158"/>
+      <c r="E1693" s="158"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19686,9 +19769,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="160"/>
-      <c r="D1710" s="161"/>
-      <c r="E1710" s="161"/>
+      <c r="C1710" s="157"/>
+      <c r="D1710" s="158"/>
+      <c r="E1710" s="158"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -19839,9 +19922,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="160"/>
-      <c r="D1727" s="161"/>
-      <c r="E1727" s="161"/>
+      <c r="C1727" s="157"/>
+      <c r="D1727" s="158"/>
+      <c r="E1727" s="158"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -19992,9 +20075,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="160"/>
-      <c r="D1744" s="161"/>
-      <c r="E1744" s="161"/>
+      <c r="C1744" s="157"/>
+      <c r="D1744" s="158"/>
+      <c r="E1744" s="158"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20145,9 +20228,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="160"/>
-      <c r="D1761" s="161"/>
-      <c r="E1761" s="161"/>
+      <c r="C1761" s="157"/>
+      <c r="D1761" s="158"/>
+      <c r="E1761" s="158"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20298,9 +20381,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="160"/>
-      <c r="D1778" s="161"/>
-      <c r="E1778" s="161"/>
+      <c r="C1778" s="157"/>
+      <c r="D1778" s="158"/>
+      <c r="E1778" s="158"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20451,9 +20534,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="160"/>
-      <c r="D1795" s="161"/>
-      <c r="E1795" s="161"/>
+      <c r="C1795" s="157"/>
+      <c r="D1795" s="158"/>
+      <c r="E1795" s="158"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20604,9 +20687,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="160"/>
-      <c r="D1812" s="161"/>
-      <c r="E1812" s="161"/>
+      <c r="C1812" s="157"/>
+      <c r="D1812" s="158"/>
+      <c r="E1812" s="158"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -20757,9 +20840,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="160"/>
-      <c r="D1829" s="161"/>
-      <c r="E1829" s="161"/>
+      <c r="C1829" s="157"/>
+      <c r="D1829" s="158"/>
+      <c r="E1829" s="158"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -20910,9 +20993,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="160"/>
-      <c r="D1846" s="161"/>
-      <c r="E1846" s="161"/>
+      <c r="C1846" s="157"/>
+      <c r="D1846" s="158"/>
+      <c r="E1846" s="158"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21063,9 +21146,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="160"/>
-      <c r="D1863" s="161"/>
-      <c r="E1863" s="161"/>
+      <c r="C1863" s="157"/>
+      <c r="D1863" s="158"/>
+      <c r="E1863" s="158"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21216,9 +21299,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="160"/>
-      <c r="D1880" s="161"/>
-      <c r="E1880" s="161"/>
+      <c r="C1880" s="157"/>
+      <c r="D1880" s="158"/>
+      <c r="E1880" s="158"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21369,9 +21452,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="160"/>
-      <c r="D1897" s="161"/>
-      <c r="E1897" s="161"/>
+      <c r="C1897" s="157"/>
+      <c r="D1897" s="158"/>
+      <c r="E1897" s="158"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21522,18 +21605,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="176"/>
-      <c r="D1914" s="177"/>
-      <c r="E1914" s="177"/>
+      <c r="C1914" s="161"/>
+      <c r="D1914" s="162"/>
+      <c r="E1914" s="162"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="160"/>
-      <c r="D1915" s="161"/>
-      <c r="E1915" s="161"/>
+      <c r="C1915" s="157"/>
+      <c r="D1915" s="158"/>
+      <c r="E1915" s="158"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21684,9 +21767,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="162"/>
-      <c r="D1932" s="163"/>
-      <c r="E1932" s="163"/>
+      <c r="C1932" s="159"/>
+      <c r="D1932" s="160"/>
+      <c r="E1932" s="160"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -21837,9 +21920,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="160"/>
-      <c r="D1949" s="161"/>
-      <c r="E1949" s="161"/>
+      <c r="C1949" s="157"/>
+      <c r="D1949" s="158"/>
+      <c r="E1949" s="158"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -21990,9 +22073,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="160"/>
-      <c r="D1966" s="161"/>
-      <c r="E1966" s="161"/>
+      <c r="C1966" s="157"/>
+      <c r="D1966" s="158"/>
+      <c r="E1966" s="158"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22143,9 +22226,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="160"/>
-      <c r="D1983" s="161"/>
-      <c r="E1983" s="161"/>
+      <c r="C1983" s="157"/>
+      <c r="D1983" s="158"/>
+      <c r="E1983" s="158"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22296,9 +22379,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="160"/>
-      <c r="D2000" s="161"/>
-      <c r="E2000" s="161"/>
+      <c r="C2000" s="157"/>
+      <c r="D2000" s="158"/>
+      <c r="E2000" s="158"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22449,9 +22532,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="160"/>
-      <c r="D2017" s="161"/>
-      <c r="E2017" s="161"/>
+      <c r="C2017" s="157"/>
+      <c r="D2017" s="158"/>
+      <c r="E2017" s="158"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22602,9 +22685,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="160"/>
-      <c r="D2034" s="161"/>
-      <c r="E2034" s="161"/>
+      <c r="C2034" s="157"/>
+      <c r="D2034" s="158"/>
+      <c r="E2034" s="158"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -22755,9 +22838,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="160"/>
-      <c r="D2051" s="161"/>
-      <c r="E2051" s="161"/>
+      <c r="C2051" s="157"/>
+      <c r="D2051" s="158"/>
+      <c r="E2051" s="158"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -22908,9 +22991,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="160"/>
-      <c r="D2068" s="161"/>
-      <c r="E2068" s="161"/>
+      <c r="C2068" s="157"/>
+      <c r="D2068" s="158"/>
+      <c r="E2068" s="158"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23061,9 +23144,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="160"/>
-      <c r="D2085" s="161"/>
-      <c r="E2085" s="161"/>
+      <c r="C2085" s="157"/>
+      <c r="D2085" s="158"/>
+      <c r="E2085" s="158"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23214,9 +23297,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="160"/>
-      <c r="D2102" s="161"/>
-      <c r="E2102" s="161"/>
+      <c r="C2102" s="157"/>
+      <c r="D2102" s="158"/>
+      <c r="E2102" s="158"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23367,9 +23450,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="160"/>
-      <c r="D2119" s="161"/>
-      <c r="E2119" s="161"/>
+      <c r="C2119" s="157"/>
+      <c r="D2119" s="158"/>
+      <c r="E2119" s="158"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23520,9 +23603,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="160"/>
-      <c r="D2136" s="161"/>
-      <c r="E2136" s="161"/>
+      <c r="C2136" s="157"/>
+      <c r="D2136" s="158"/>
+      <c r="E2136" s="158"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23673,9 +23756,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="160"/>
-      <c r="D2153" s="161"/>
-      <c r="E2153" s="161"/>
+      <c r="C2153" s="157"/>
+      <c r="D2153" s="158"/>
+      <c r="E2153" s="158"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -23826,9 +23909,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="160"/>
-      <c r="D2170" s="161"/>
-      <c r="E2170" s="161"/>
+      <c r="C2170" s="157"/>
+      <c r="D2170" s="158"/>
+      <c r="E2170" s="158"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -23976,15 +24059,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -23997,124 +24187,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24865,7 +24948,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25076,7 +25159,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25206,9 +25289,9 @@
       <c r="B11" s="131" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="130">
+      <c r="C11" s="130" t="str">
         <f>FrameCounts!B11</f>
-        <v>0</v>
+        <v>Title screen end</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -25218,9 +25301,9 @@
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="132">
+      <c r="C12" s="132" t="str">
         <f>FrameCounts!B12</f>
-        <v>0</v>
+        <v>End map</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -25296,9 +25379,9 @@
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="132">
-        <f>FrameCounts!B21</f>
-        <v>0</v>
+      <c r="C20" s="132" t="str">
+        <f>FrameCounts!B22</f>
+        <v>Level 1 Begin</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
@@ -25314,7 +25397,7 @@
         <v>212</v>
       </c>
       <c r="C22" s="134">
-        <f>FrameCounts!H20</f>
+        <f>FrameCounts!H21</f>
         <v>0</v>
       </c>
     </row>
@@ -25349,7 +25432,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25371,150 +25454,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="202" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="199" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="210"/>
+      <c r="B2" s="200"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="210"/>
+      <c r="B3" s="200"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="205" t="s">
+      <c r="A5" s="204" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="206"/>
+      <c r="B5" s="205"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="210" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="198"/>
+      <c r="B7" s="211"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="208" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="200"/>
+      <c r="B9" s="209"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202"/>
+      <c r="A10" s="195"/>
+      <c r="B10" s="196"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="194"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="194"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="194"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="194"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="194"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="193" t="s">
+      <c r="A16" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="194"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="193" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="196"/>
+      <c r="B17" s="194"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="210" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="198"/>
+      <c r="B19" s="211"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="199" t="s">
+      <c r="A21" s="208" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="200"/>
+      <c r="B21" s="209"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="201"/>
-      <c r="B22" s="202"/>
+      <c r="A22" s="195"/>
+      <c r="B22" s="196"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="193" t="s">
+      <c r="A23" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="194"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="193"/>
-      <c r="B24" s="194"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="194"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="193" t="s">
+      <c r="A26" s="197" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="194"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="193"/>
+      <c r="B27" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25525,19 +25621,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>